<commit_message>
example code for manuscript
</commit_message>
<xml_diff>
--- a/data/codebook-main-step2step3-sample-without-results.xlsx
+++ b/data/codebook-main-step2step3-sample-without-results.xlsx
@@ -4093,7 +4093,7 @@
         </is>
       </c>
       <c r="AM36">
-        <v>946</v>
+        <v>945</v>
       </c>
     </row>
     <row r="37">
@@ -4198,7 +4198,7 @@
         </is>
       </c>
       <c r="AM37">
-        <v>1136</v>
+        <v>1134</v>
       </c>
     </row>
     <row r="38">
@@ -4342,7 +4342,7 @@
         </is>
       </c>
       <c r="AM38">
-        <v>1146</v>
+        <v>1144</v>
       </c>
     </row>
     <row r="39">
@@ -4486,7 +4486,7 @@
         </is>
       </c>
       <c r="AM39">
-        <v>1147</v>
+        <v>1145</v>
       </c>
     </row>
     <row r="40">
@@ -4630,7 +4630,7 @@
         </is>
       </c>
       <c r="AM40">
-        <v>1148</v>
+        <v>1146</v>
       </c>
     </row>
     <row r="41">
@@ -4774,7 +4774,7 @@
         </is>
       </c>
       <c r="AM41">
-        <v>1149</v>
+        <v>1147</v>
       </c>
     </row>
     <row r="42">
@@ -4918,7 +4918,7 @@
         </is>
       </c>
       <c r="AM42">
-        <v>1150</v>
+        <v>1148</v>
       </c>
     </row>
   </sheetData>

</xml_diff>